<commit_message>
erste Ideen in Brainstorming muss noch schön gemacht werden
</commit_message>
<xml_diff>
--- a/Brainstorming.xlsx
+++ b/Brainstorming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niels\Desktop\Smart-Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{374F628B-8D74-4A4B-8B09-266BD946B92C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E958B0EF-3654-45C4-88B4-40C4027AD27C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3580" xr2:uid="{4D016826-7E4A-4565-B8F8-48E7756074D0}"/>
   </bookViews>
@@ -22,6 +22,62 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Magic Mirror</t>
+  </si>
+  <si>
+    <t>Phone Control</t>
+  </si>
+  <si>
+    <t>Heizung  Licht</t>
+  </si>
+  <si>
+    <t>automatisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tür licht an </t>
+  </si>
+  <si>
+    <t>licht aus</t>
+  </si>
+  <si>
+    <t>alexa</t>
+  </si>
+  <si>
+    <t>Tisch hoch runter fahren</t>
+  </si>
+  <si>
+    <t>kalender</t>
+  </si>
+  <si>
+    <t>wetter</t>
+  </si>
+  <si>
+    <t>news</t>
+  </si>
+  <si>
+    <t>mit eigenen mess daten</t>
+  </si>
+  <si>
+    <t>farbiges licht</t>
+  </si>
+  <si>
+    <t>touch face recognicion</t>
+  </si>
+  <si>
+    <t>raspberry pi 4</t>
+  </si>
+  <si>
+    <t>(iPad?)</t>
+  </si>
+  <si>
+    <t>rolläden</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,12 +427,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF28471-F51F-4E0D-A1D7-F70B6C39D48A}">
-  <dimension ref="A1"/>
+  <dimension ref="B4:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.6328125" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
erste recherche zu raspi
</commit_message>
<xml_diff>
--- a/Brainstorming.xlsx
+++ b/Brainstorming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niels\Desktop\Smart-Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E958B0EF-3654-45C4-88B4-40C4027AD27C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5310B46-AD5D-4E08-BB5D-82A7EDF71ED5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3580" xr2:uid="{4D016826-7E4A-4565-B8F8-48E7756074D0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Magic Mirror</t>
   </si>
@@ -76,16 +76,97 @@
   </si>
   <si>
     <t>rolläden</t>
+  </si>
+  <si>
+    <t>Parts</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 4</t>
+  </si>
+  <si>
+    <t>Pi Camera Module</t>
+  </si>
+  <si>
+    <t>Pi Case</t>
+  </si>
+  <si>
+    <t>Micro SD Card (32 GB)</t>
+  </si>
+  <si>
+    <t>SD Card Adaptor</t>
+  </si>
+  <si>
+    <t>Alexa</t>
+  </si>
+  <si>
+    <t>HDMI-Kabel (Micro)</t>
+  </si>
+  <si>
+    <t>Pi 4 Charger</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>41.77€</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/-/en/Raspberry-ARM-Cortex-A72-4x1-50GHz-WLANac-Bluetooth/dp/B07TD42S27/ref=sr_1_4?dchild=1&amp;keywords=raspberry+pi+4&amp;qid=1602619672&amp;quartzVehicle=812-409&amp;replacementKeywords=raspberry+pi&amp;sr=8-4</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/-/en/Raspberry-V2-0-1080P-Camera-Module/dp/B07VRJKYYB/ref=sr_1_4?camp=1789&amp;creative=9325&amp;creativeASIN=B01ER2SKFS&amp;dchild=1&amp;keywords=Raspberry+Pi+Camera+Module+V2-8+Megapixel%2C1080p+%28RPI-CAM-V2%29&amp;linkCode=gs3&amp;linkId=6046a185cff8e8f9d17c96c0dc423054&amp;qid=1602619865&amp;sr=8-4&amp;tag=sbio200b-21</t>
+  </si>
+  <si>
+    <t>27.99€</t>
+  </si>
+  <si>
+    <t>8.53€</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/Snowkids-HDMI-Cable-grey/dp/B07Z838XB3/ref=sr_1_1_sspa?crid=F7NU7MW3A1KA&amp;dchild=1&amp;keywords=micro+hdmi+auf+hdmi&amp;qid=1602620021&amp;s=industrial&amp;sprefix=micr+hdmi%2Cindustrial%2C194&amp;sr=1-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyNzQ2R1NMTlI1RzE2JmVuY3J5cHRlZElkPUEwMjQ1NjczNFU1VVo5RlpHTzBKJmVuY3J5cHRlZEFkSWQ9QTAyMDg1MjhGSDEyU1dGQkVGUkomd2lkZ2V0TmFtZT1zcF9hdGYmYWN0aW9uPWNsaWNrUmVkaXJlY3QmZG9Ob3RMb2dDbGljaz10cnVl</t>
+  </si>
+  <si>
+    <t>6.49€</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/-/en/SanDisk-Ultra-microSDHC-memory-adapter/dp/B073JWXGNT/ref=sr_1_3?dchild=1&amp;keywords=micro+sd+32gb&amp;qid=1602620142&amp;s=computers&amp;sr=1-3</t>
+  </si>
+  <si>
+    <t>99.99€</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Two-Way-Glass-Mirror-Surveillance/dp/B01MSAZ3PN/ref=sr_1_2?dchild=1&amp;keywords=two%2Bway%2Bmirror&amp;linkCode=sl2&amp;linkId=7e6a999ff9359db56792d791cb4ff51f&amp;qid=1602620232&amp;sr=8-2&amp;tag=sbio20-20&amp;th=1</t>
+  </si>
+  <si>
+    <t>14.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,13 +189,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -427,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF28471-F51F-4E0D-A1D7-F70B6C39D48A}">
-  <dimension ref="B4:J11"/>
+  <dimension ref="B4:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,7 +592,103 @@
         <v>14</v>
       </c>
     </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G24" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E17" r:id="rId1" display="https://www.amazon.de/Snowkids-HDMI-Cable-grey/dp/B07Z838XB3/ref=sr_1_1_sspa?crid=F7NU7MW3A1KA&amp;dchild=1&amp;keywords=micro+hdmi+auf+hdmi&amp;qid=1602620021&amp;s=industrial&amp;sprefix=micr+hdmi%2Cindustrial%2C194&amp;sr=1-1-spons&amp;psc=1&amp;spLa=ZW5jcnlwdGVkUXVhbGlmaWVyPUEyNzQ2R1NMTlI1RzE2JmVuY3J5cHRlZElkPUEwMjQ1NjczNFU1VVo5RlpHTzBKJmVuY3J5cHRlZEFkSWQ9QTAyMDg1MjhGSDEyU1dGQkVGUkomd2lkZ2V0TmFtZT1zcF9hdGYmYWN0aW9uPWNsaWNrUmVkaXJlY3QmZG9Ob3RMb2dDbGljaz10cnVl" xr:uid="{8D7840AC-F2A2-45FF-AFCF-AEA9901B0FD5}"/>
+    <hyperlink ref="E16" r:id="rId2" display="https://www.amazon.de/-/en/Raspberry-V2-0-1080P-Camera-Module/dp/B07VRJKYYB/ref=sr_1_4?camp=1789&amp;creative=9325&amp;creativeASIN=B01ER2SKFS&amp;dchild=1&amp;keywords=Raspberry+Pi+Camera+Module+V2-8+Megapixel%2C1080p+%28RPI-CAM-V2%29&amp;linkCode=gs3&amp;linkId=6046a185cff8e8f9d17c96c0dc423054&amp;qid=1602619865&amp;sr=8-4&amp;tag=sbio200b-21" xr:uid="{5C0D83CF-C145-4919-98F0-23271A098F55}"/>
+    <hyperlink ref="E15" r:id="rId3" xr:uid="{2416325F-CE10-44F3-95A9-FFD9C8D0AF8B}"/>
+    <hyperlink ref="E18" r:id="rId4" xr:uid="{F18567BB-721A-49B6-B27D-F950B771D0AE}"/>
+    <hyperlink ref="E19" r:id="rId5" xr:uid="{D6D43874-0200-4F58-ADF3-724D2C0049FF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>